<commit_message>
WiP ControlledGasBoiler momentum validated
</commit_message>
<xml_diff>
--- a/doc/teorethicalcomputation4tests.xlsx
+++ b/doc/teorethicalcomputation4tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DiscoD\Muro\GitHub\multienergysystem\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AC8E892-BA22-40E3-8031-C10E1BA7A630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{85707EDF-63A2-4AFE-8B41-5E7C163227A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{48B1869B-21F5-4BDF-B69D-8E219112A809}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{48B1869B-21F5-4BDF-B69D-8E219112A809}"/>
   </bookViews>
   <sheets>
     <sheet name="Mass_Energy Balance" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="HeatPumps" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="56">
   <si>
     <t>HX01</t>
   </si>
@@ -204,6 +205,9 @@
   </si>
   <si>
     <t>dp (Pa)</t>
+  </si>
+  <si>
+    <t>dp (bar)</t>
   </si>
 </sst>
 </file>
@@ -446,48 +450,66 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Only Boiler'!$AN$56:$AN$60</c:f>
+              <c:f>'Only Boiler'!$AN$56:$AN$63</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>1.925</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>3.5750000000000002</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>4.95</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>6.05</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>9.35</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.45</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Only Boiler'!$AO$56:$AO$60</c:f>
+              <c:f>'Only Boiler'!$AO$56:$AO$63</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>980.66499999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>1961.33</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>2941.9949999999999</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>3922.66</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>7845.32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9316.3174999999992</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10051.816249999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1283,16 +1305,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>126223</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>38158</xdr:rowOff>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>453472</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>115423</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>413547</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>51908</xdr:rowOff>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>134660</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>125177</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2208,10 +2230,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0539F5BB-28F8-4AFC-BFAF-78EBA52576BB}">
-  <dimension ref="C5:AO60"/>
+  <dimension ref="C5:AP63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AF40" sqref="AF40"/>
+    <sheetView tabSelected="1" topLeftCell="J8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AX69" sqref="AX69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3299,7 +3321,7 @@
         <v>100.26266540000009</v>
       </c>
     </row>
-    <row r="55" spans="38:41" x14ac:dyDescent="0.3">
+    <row r="55" spans="38:42" x14ac:dyDescent="0.3">
       <c r="AL55" t="s">
         <v>51</v>
       </c>
@@ -3312,8 +3334,11 @@
       <c r="AO55" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="56" spans="38:41" x14ac:dyDescent="0.3">
+      <c r="AP55" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="56" spans="38:42" x14ac:dyDescent="0.3">
       <c r="AL56">
         <v>0</v>
       </c>
@@ -3321,76 +3346,156 @@
         <v>0</v>
       </c>
       <c r="AN56">
-        <f>+AL56*990/3600</f>
+        <f t="shared" ref="AN56:AN63" si="2">+AL56*990/3600</f>
         <v>0</v>
       </c>
       <c r="AO56">
-        <f>+AM56*9806.65</f>
+        <f t="shared" ref="AO56:AO63" si="3">+AM56*9806.65</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="38:41" x14ac:dyDescent="0.3">
+      <c r="AP56">
+        <f>+AO56/100000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="38:42" x14ac:dyDescent="0.3">
       <c r="AL57">
+        <v>7</v>
+      </c>
+      <c r="AM57">
+        <v>0.1</v>
+      </c>
+      <c r="AN57">
+        <f t="shared" si="2"/>
+        <v>1.925</v>
+      </c>
+      <c r="AO57">
+        <f t="shared" si="3"/>
+        <v>980.66499999999996</v>
+      </c>
+      <c r="AP57">
+        <f t="shared" ref="AP57:AP63" si="4">+AO57/100000</f>
+        <v>9.8066500000000001E-3</v>
+      </c>
+    </row>
+    <row r="58" spans="38:42" x14ac:dyDescent="0.3">
+      <c r="AL58">
         <v>13</v>
       </c>
-      <c r="AM57">
+      <c r="AM58">
         <v>0.2</v>
       </c>
-      <c r="AN57">
-        <f>+AL57*990/3600</f>
+      <c r="AN58">
+        <f t="shared" si="2"/>
         <v>3.5750000000000002</v>
       </c>
-      <c r="AO57">
-        <f>+AM57*9806.65</f>
+      <c r="AO58">
+        <f t="shared" si="3"/>
         <v>1961.33</v>
       </c>
-    </row>
-    <row r="58" spans="38:41" x14ac:dyDescent="0.3">
-      <c r="AL58">
+      <c r="AP58">
+        <f t="shared" si="4"/>
+        <v>1.96133E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="38:42" x14ac:dyDescent="0.3">
+      <c r="AL59">
         <v>18</v>
       </c>
-      <c r="AM58">
+      <c r="AM59">
         <v>0.3</v>
       </c>
-      <c r="AN58">
-        <f>+AL58*990/3600</f>
+      <c r="AN59">
+        <f t="shared" si="2"/>
         <v>4.95</v>
       </c>
-      <c r="AO58">
-        <f>+AM58*9806.65</f>
+      <c r="AO59">
+        <f t="shared" si="3"/>
         <v>2941.9949999999999</v>
       </c>
-    </row>
-    <row r="59" spans="38:41" x14ac:dyDescent="0.3">
-      <c r="AL59">
+      <c r="AP59">
+        <f t="shared" si="4"/>
+        <v>2.941995E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="38:42" x14ac:dyDescent="0.3">
+      <c r="AL60">
         <v>22</v>
       </c>
-      <c r="AM59">
+      <c r="AM60">
         <v>0.4</v>
       </c>
-      <c r="AN59">
-        <f>+AL59*990/3600</f>
+      <c r="AN60">
+        <f t="shared" si="2"/>
         <v>6.05</v>
       </c>
-      <c r="AO59">
-        <f>+AM59*9806.65</f>
+      <c r="AO60">
+        <f t="shared" si="3"/>
         <v>3922.66</v>
       </c>
-    </row>
-    <row r="60" spans="38:41" x14ac:dyDescent="0.3">
-      <c r="AL60">
+      <c r="AP60">
+        <f t="shared" si="4"/>
+        <v>3.92266E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="38:42" x14ac:dyDescent="0.3">
+      <c r="AL61">
         <v>34</v>
       </c>
-      <c r="AM60">
+      <c r="AM61">
         <v>0.8</v>
       </c>
-      <c r="AN60">
-        <f>+AL60*990/3600</f>
+      <c r="AN61">
+        <f t="shared" si="2"/>
         <v>9.35</v>
       </c>
-      <c r="AO60">
-        <f>+AM60*9806.65</f>
+      <c r="AO61">
+        <f t="shared" si="3"/>
         <v>7845.32</v>
+      </c>
+      <c r="AP61">
+        <f t="shared" si="4"/>
+        <v>7.8453200000000001E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="38:42" x14ac:dyDescent="0.3">
+      <c r="AL62">
+        <v>38</v>
+      </c>
+      <c r="AM62">
+        <v>0.95</v>
+      </c>
+      <c r="AN62">
+        <f t="shared" si="2"/>
+        <v>10.45</v>
+      </c>
+      <c r="AO62">
+        <f t="shared" si="3"/>
+        <v>9316.3174999999992</v>
+      </c>
+      <c r="AP62">
+        <f t="shared" si="4"/>
+        <v>9.3163174999999987E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="38:42" x14ac:dyDescent="0.3">
+      <c r="AL63">
+        <v>40</v>
+      </c>
+      <c r="AM63">
+        <v>1.0249999999999999</v>
+      </c>
+      <c r="AN63">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="AO63">
+        <f t="shared" si="3"/>
+        <v>10051.816249999998</v>
+      </c>
+      <c r="AP63">
+        <f t="shared" si="4"/>
+        <v>0.10051816249999998</v>
       </c>
     </row>
   </sheetData>
@@ -5108,11 +5213,11 @@
         <v>48.920454545454547</v>
       </c>
       <c r="M16">
-        <f t="shared" ref="M16:N16" si="0">+M12</f>
+        <f>+M12</f>
         <v>45</v>
       </c>
       <c r="N16">
-        <f t="shared" si="0"/>
+        <f>+N12</f>
         <v>2.4444444444444446</v>
       </c>
       <c r="P16">

</xml_diff>